<commit_message>
Changes done by Rashmi
</commit_message>
<xml_diff>
--- a/Data Files/Excel_Files/FP_Details.xlsx
+++ b/Data Files/Excel_Files/FP_Details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJT_Katalon\NJTRANSIT_Web_Maintinace\Data Files\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJT_Katalon_Automation_May\NJTRANSIT_Web\Data Files\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E330C3-0D49-4F1B-87F4-B554230FE49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A998DC9-E34A-481F-A572-BC0B5D46DA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>FP_Card_No</t>
   </si>
   <si>
     <t>FP_Pin</t>
-  </si>
-  <si>
-    <t>6375004107031383</t>
   </si>
   <si>
     <t>6375004102003502</t>
@@ -375,7 +372,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,15 +390,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>225</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>571</v>
@@ -409,7 +406,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>959</v>
@@ -417,7 +414,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>779</v>
@@ -425,7 +422,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>257</v>

</xml_diff>

<commit_message>
New_Regression test suite added for failed test cases from c3 by Mythreye on June 6th at 1:35 PM
</commit_message>
<xml_diff>
--- a/Data Files/Excel_Files/FP_Details.xlsx
+++ b/Data Files/Excel_Files/FP_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJT_Katalon_Automation_May\NJTRANSIT_Web\Data Files\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJTAutomation\NJT_WEB_c.3\NJTRANSIT\Data Files\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A998DC9-E34A-481F-A572-BC0B5D46DA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17044E2F-C9A7-443C-A888-510F99445AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>FP_Card_No</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>6375004102254139</t>
+  </si>
+  <si>
+    <t>6375004107031383</t>
   </si>
 </sst>
 </file>
@@ -61,15 +64,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,17 +86,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,7 +402,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,11 +435,11 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>959</v>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>